<commit_message>
Added the new button 13-17 on app
</commit_message>
<xml_diff>
--- a/Buttons Testing Table.xlsx
+++ b/Buttons Testing Table.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stelios\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Stelios\Desktop\SDP\SDP-2018\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5FBDE56E-EFEC-4BAA-B57F-859D58EE1D6B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB6D549A-F155-4B5A-B1C2-D14B0C32AD92}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{F613F66A-5BDC-4DBD-9703-E92288479E80}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="33">
   <si>
     <t>Say Hello</t>
   </si>
@@ -120,13 +120,10 @@
     <t>?</t>
   </si>
   <si>
-    <t>ERROR DURING GAME</t>
-  </si>
-  <si>
-    <t xml:space="preserve">*graph on phone doesn't display all 12 values </t>
-  </si>
-  <si>
-    <t>* Have not checked the LEDs</t>
+    <t xml:space="preserve">PHONE CRASHES SOMETIMES </t>
+  </si>
+  <si>
+    <t>Leds working Okay</t>
   </si>
 </sst>
 </file>
@@ -614,7 +611,7 @@
   <dimension ref="A3:I29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -683,8 +680,12 @@
       <c r="B6" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
+      <c r="C6" s="1">
+        <v>13</v>
+      </c>
+      <c r="D6" s="1">
+        <v>13</v>
+      </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
@@ -696,8 +697,12 @@
       <c r="B7" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
+      <c r="C7" s="1">
+        <v>14</v>
+      </c>
+      <c r="D7" s="1">
+        <v>14</v>
+      </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -709,8 +714,12 @@
       <c r="B8" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
+      <c r="C8" s="1">
+        <v>15</v>
+      </c>
+      <c r="D8" s="1">
+        <v>15</v>
+      </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -722,8 +731,12 @@
       <c r="B9" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
+      <c r="C9" s="1">
+        <v>16</v>
+      </c>
+      <c r="D9" s="1">
+        <v>16</v>
+      </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -735,8 +748,12 @@
       <c r="B10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
+      <c r="C10" s="1">
+        <v>17</v>
+      </c>
+      <c r="D10" s="1">
+        <v>17</v>
+      </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
       <c r="G10" s="1"/>
@@ -760,7 +777,7 @@
         <v>29</v>
       </c>
       <c r="H11" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I11" s="9"/>
     </row>
@@ -896,9 +913,11 @@
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H18" s="9"/>
+        <v>29</v>
+      </c>
+      <c r="H18" s="9">
+        <v>6</v>
+      </c>
       <c r="I18" s="9"/>
     </row>
     <row r="19" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -917,9 +936,11 @@
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H19" s="9"/>
+        <v>29</v>
+      </c>
+      <c r="H19" s="9">
+        <v>6</v>
+      </c>
       <c r="I19" s="9"/>
     </row>
     <row r="20" spans="1:9" ht="15.6" x14ac:dyDescent="0.3">
@@ -940,8 +961,8 @@
       <c r="G20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="H20" s="9" t="s">
-        <v>32</v>
+      <c r="H20" s="9">
+        <v>12</v>
       </c>
       <c r="I20" s="9"/>
     </row>
@@ -961,7 +982,7 @@
       </c>
       <c r="F21" s="3"/>
       <c r="G21" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>

</xml_diff>